<commit_message>
change file extension to tsv
</commit_message>
<xml_diff>
--- a/messy-project-directory/Survey Data_clean.xlsx
+++ b/messy-project-directory/Survey Data_clean.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carac\Documents\UW MCB PhD\Computational Tools\tfcb_homework02\tfcb-homework02\messy-project-directory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5248F27B-F10F-42D8-A758-1E565E79ABBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03BFA290-60C8-480A-8A3D-083264F0E6F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="481" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,9 +75,6 @@
     <t>2013-07-17</t>
   </si>
   <si>
-    <t xml:space="preserve">Weight (g) (calibrated) </t>
-  </si>
-  <si>
     <t>2013-08-19</t>
   </si>
   <si>
@@ -151,6 +148,9 @@
   </si>
   <si>
     <t>* indicates data not calibrated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weight (g) </t>
   </si>
 </sst>
 </file>
@@ -604,7 +604,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -648,7 +648,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -672,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83990D8B-2392-4656-AC03-C630F945A319}">
   <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="88" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -681,7 +681,7 @@
     <col min="1" max="1" width="4.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.21875" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -698,7 +698,7 @@
         <v>9</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -715,7 +715,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -723,7 +723,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
@@ -740,7 +740,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>2</v>
@@ -757,7 +757,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>2</v>
@@ -774,7 +774,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>2</v>
@@ -791,7 +791,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>2</v>
@@ -808,7 +808,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>5</v>
@@ -834,7 +834,7 @@
         <v>3</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="3"/>
@@ -848,16 +848,16 @@
         <v>2</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="3"/>
@@ -871,7 +871,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>2</v>
@@ -894,7 +894,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>4</v>
@@ -917,7 +917,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>2</v>
@@ -940,16 +940,16 @@
         <v>2</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="3"/>
@@ -963,7 +963,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>5</v>
@@ -972,7 +972,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="3"/>
@@ -986,16 +986,16 @@
         <v>2</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="3"/>
@@ -1009,7 +1009,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>0</v>
@@ -1018,7 +1018,7 @@
         <v>1</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I17" s="1"/>
       <c r="J17" s="3"/>
@@ -1032,7 +1032,7 @@
         <v>2</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>4</v>
@@ -1055,7 +1055,7 @@
         <v>2</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>2</v>
@@ -1087,7 +1087,7 @@
         <v>1</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I20" s="1"/>
       <c r="J20" s="3"/>
@@ -1124,7 +1124,7 @@
         <v>3</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>12</v>
@@ -1147,7 +1147,7 @@
         <v>3</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>12</v>
@@ -1170,7 +1170,7 @@
         <v>3</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>4</v>
@@ -1193,7 +1193,7 @@
         <v>3</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>0</v>
@@ -1202,7 +1202,7 @@
         <v>3</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I25" s="1"/>
       <c r="J25" s="3"/>
@@ -1216,16 +1216,16 @@
         <v>3</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I26" s="1"/>
       <c r="J26" s="3"/>
@@ -1239,7 +1239,7 @@
         <v>3</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>0</v>
@@ -1262,7 +1262,7 @@
         <v>3</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>6</v>
@@ -1285,7 +1285,7 @@
         <v>3</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>0</v>
@@ -1308,7 +1308,7 @@
         <v>3</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>0</v>
@@ -1331,7 +1331,7 @@
         <v>4</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>2</v>
@@ -1354,7 +1354,7 @@
         <v>4</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>2</v>
@@ -1363,7 +1363,7 @@
         <v>1</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I32" s="1"/>
       <c r="J32" s="3"/>
@@ -1377,7 +1377,7 @@
         <v>4</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>2</v>
@@ -1400,7 +1400,7 @@
         <v>4</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>12</v>
@@ -1423,10 +1423,10 @@
         <v>4</v>
       </c>
       <c r="B35" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>1</v>
@@ -1463,7 +1463,7 @@
         <v>4</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>5</v>
@@ -1480,7 +1480,7 @@
         <v>4</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>5</v>
@@ -1548,7 +1548,7 @@
         <v>8</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>12</v>
@@ -1565,7 +1565,7 @@
         <v>8</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>12</v>
@@ -1582,7 +1582,7 @@
         <v>9</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>5</v>
@@ -1599,7 +1599,7 @@
         <v>9</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>12</v>
@@ -1616,7 +1616,7 @@
         <v>11</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>5</v>
@@ -1633,7 +1633,7 @@
         <v>11</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>5</v>
@@ -1650,7 +1650,7 @@
         <v>14</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>5</v>
@@ -1659,7 +1659,7 @@
         <v>1</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1667,7 +1667,7 @@
         <v>17</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>5</v>
@@ -1676,7 +1676,7 @@
         <v>3</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1688,12 +1688,12 @@
     </row>
     <row r="51" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B52" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>